<commit_message>
Added strategies to control the process data flow of PortController. Refactorized PortController code.
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,351 +434,53 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>measure 1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>measure 2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>measure 3</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>measure 4</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>measure 5</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>measure 6</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>measure 7</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>measure 8</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>measure 9</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>measure 10</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="A2" t="n">
+        <v>53</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5</v>
-      </c>
-      <c r="H2" t="n">
-        <v>6</v>
-      </c>
-      <c r="I2" t="n">
-        <v>7</v>
-      </c>
-      <c r="J2" t="n">
-        <v>8</v>
-      </c>
-      <c r="K2" t="n">
-        <v>9</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A3" t="n">
+        <v>54</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H3" t="n">
-        <v>12</v>
-      </c>
-      <c r="I3" t="n">
-        <v>14</v>
-      </c>
-      <c r="J3" t="n">
-        <v>16</v>
-      </c>
-      <c r="K3" t="n">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A4" t="n">
+        <v>52</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>9</v>
-      </c>
-      <c r="F4" t="n">
-        <v>12</v>
-      </c>
-      <c r="G4" t="n">
-        <v>15</v>
-      </c>
-      <c r="H4" t="n">
-        <v>18</v>
-      </c>
-      <c r="I4" t="n">
-        <v>21</v>
-      </c>
-      <c r="J4" t="n">
-        <v>24</v>
-      </c>
-      <c r="K4" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F5" t="n">
-        <v>16</v>
-      </c>
-      <c r="G5" t="n">
-        <v>20</v>
-      </c>
-      <c r="H5" t="n">
-        <v>24</v>
-      </c>
-      <c r="I5" t="n">
-        <v>28</v>
-      </c>
-      <c r="J5" t="n">
-        <v>32</v>
-      </c>
-      <c r="K5" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" t="n">
-        <v>20</v>
-      </c>
-      <c r="G6" t="n">
-        <v>25</v>
-      </c>
-      <c r="H6" t="n">
-        <v>30</v>
-      </c>
-      <c r="I6" t="n">
-        <v>35</v>
-      </c>
-      <c r="J6" t="n">
-        <v>40</v>
-      </c>
-      <c r="K6" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" t="n">
-        <v>12</v>
-      </c>
-      <c r="E7" t="n">
-        <v>18</v>
-      </c>
-      <c r="F7" t="n">
-        <v>24</v>
-      </c>
-      <c r="G7" t="n">
-        <v>30</v>
-      </c>
-      <c r="H7" t="n">
-        <v>36</v>
-      </c>
-      <c r="I7" t="n">
-        <v>42</v>
-      </c>
-      <c r="J7" t="n">
-        <v>48</v>
-      </c>
-      <c r="K7" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>7</v>
-      </c>
-      <c r="D8" t="n">
-        <v>14</v>
-      </c>
-      <c r="E8" t="n">
-        <v>21</v>
-      </c>
-      <c r="F8" t="n">
-        <v>28</v>
-      </c>
-      <c r="G8" t="n">
-        <v>35</v>
-      </c>
-      <c r="H8" t="n">
-        <v>42</v>
-      </c>
-      <c r="I8" t="n">
-        <v>49</v>
-      </c>
-      <c r="J8" t="n">
-        <v>56</v>
-      </c>
-      <c r="K8" t="n">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>8</v>
-      </c>
-      <c r="D9" t="n">
-        <v>16</v>
-      </c>
-      <c r="E9" t="n">
-        <v>24</v>
-      </c>
-      <c r="F9" t="n">
-        <v>32</v>
-      </c>
-      <c r="G9" t="n">
-        <v>40</v>
-      </c>
-      <c r="H9" t="n">
-        <v>48</v>
-      </c>
-      <c r="I9" t="n">
-        <v>56</v>
-      </c>
-      <c r="J9" t="n">
-        <v>64</v>
-      </c>
-      <c r="K9" t="n">
-        <v>72</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>